<commit_message>
add check term change(not complete)
</commit_message>
<xml_diff>
--- a/public/Datatest.xlsx
+++ b/public/Datatest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projectWeb\node_plan\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9AAE89-278C-4D19-8B99-06151F7F01DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579304D3-ECFF-434A-8E8A-DD9A3C612432}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AEC55A8B-6158-476E-81E6-CA07EB20D31A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="184">
   <si>
     <t>ID</t>
   </si>
@@ -583,6 +583,9 @@
   </si>
   <si>
     <t>1 in CPE332</t>
+  </si>
+  <si>
+    <t>7/2</t>
   </si>
 </sst>
 </file>
@@ -977,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276D5559-B1B8-4541-89FA-2D757767FB71}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="23.4"/>
@@ -1354,7 +1357,7 @@
         <v>3</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>25</v>
+        <v>183</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>140</v>

</xml_diff>